<commit_message>
Added two new fields to NSDE: `inactivation_date` and `reactivation_date`.
</commit_message>
<xml_diff>
--- a/static/fields/othernsde_reference.xlsx
+++ b/static/fields/othernsde_reference.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denis.krylov/Projects/openFDA/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FCBA87-9D36-434E-A6C2-329BBED48A4B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434ACC9B-9D6E-2542-8CE2-57DB91E79C0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="760" windowWidth="26540" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38160" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="device_classification_fields" sheetId="1" r:id="rId1"/>
+    <sheet name="nsde_fields" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Field Name</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>The National Council for Prescription Drug Programs (NCPDP) developed the Billing Unit Standard to assist in consistent and accurate billing of pharmaceutical products. Information on the NCPDP Billing Unit Standard may be found at http://www.ncpdp.org/PDF/BUS_overview.pdfdisclaimer icon. This column may contain a NCPDP Billing Unit (GM, ML or EA).</t>
+  </si>
+  <si>
+    <t>inactivation_date</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>The date on which registration or listing data was inactivated by FDA due to inaccuracies, incompleteness or incompliance.</t>
+  </si>
+  <si>
+    <t>reactivation_date</t>
+  </si>
+  <si>
+    <t>The date on which a previously FDA inactivated registration or listing data is reactivated.</t>
   </si>
 </sst>
 </file>
@@ -379,7 +394,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -399,6 +414,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="215">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -955,18 +971,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.5" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -1092,6 +1108,28 @@
       </c>
       <c r="D11" s="5" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>